<commit_message>
Updated code to support new prompt template with following features: hallucination guardrails, support manual role assignment, run test mode on all treatments, response choice order randomisation, task order randomisation, summarizer agent, manual turn-based flow, and different action spaces for each role.
</commit_message>
<xml_diff>
--- a/demos/public_good_experiment_prompt_template.xlsx
+++ b/demos/public_good_experiment_prompt_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondlow/Documents/talking-to-machines/talking-to-machines/demos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A204DCF7-16F0-0B4E-91FA-01DA3891A652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2935FD-A2A9-FF46-B73D-817761ED936B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-23280" windowWidth="34560" windowHeight="22340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experimental_setting" sheetId="1" r:id="rId1"/>
     <sheet name="treatments" sheetId="2" r:id="rId2"/>
     <sheet name="agent_roles" sheetId="3" r:id="rId3"/>
-    <sheet name="prompts_template" sheetId="4" r:id="rId4"/>
+    <sheet name="interview_prompts" sheetId="4" r:id="rId4"/>
     <sheet name="agent_profiles" sheetId="5" r:id="rId5"/>
     <sheet name="constants" sheetId="6" r:id="rId6"/>
   </sheets>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Assume the role of a facilitator in a public good experiment.</t>
-  </si>
-  <si>
-    <t>Summariser</t>
   </si>
   <si>
     <t>Assume the role of a summariser in a public good experiment involving 4 participants. Each participant will start with an initial endowment of 10 tokens. During each round of the experiment, each participant is asked to decide how many tokens to contribute to a public account and how many to keep in their private account. The tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in the participants' private account will not be shared and remain private. 
@@ -455,6 +452,9 @@
   <si>
     <t>treatment_column</t>
   </si>
+  <si>
+    <t>Summarizer</t>
+  </si>
 </sst>
 </file>
 
@@ -772,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -846,7 +846,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>16</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" s="4">
         <v>42</v>
@@ -2932,7 +2932,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2960,42 +2962,42 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4005,7 +4007,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB858"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4025,40 +4029,40 @@
   <sheetData>
     <row r="1" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="M1" s="6"/>
       <c r="N1" s="8"/>
@@ -4082,7 +4086,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -4091,13 +4095,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -4132,7 +4136,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -4141,19 +4145,19 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="J3" s="6">
         <v>1</v>
@@ -4186,7 +4190,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -4195,19 +4199,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="J4" s="6">
         <v>1</v>
@@ -4240,7 +4244,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -4249,19 +4253,19 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J5" s="6">
         <v>1</v>
@@ -4294,7 +4298,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3">
         <v>4</v>
@@ -4303,19 +4307,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="J6" s="6">
         <v>0</v>
@@ -4348,7 +4352,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3">
         <v>4</v>
@@ -4357,19 +4361,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="J7" s="6">
         <v>0</v>
@@ -4402,7 +4406,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3">
         <v>4</v>
@@ -4411,19 +4415,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="J8" s="6">
         <v>0</v>
@@ -4456,7 +4460,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3">
         <v>4</v>
@@ -4465,19 +4469,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="6">
         <v>0</v>
@@ -4510,7 +4514,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3">
         <v>4</v>
@@ -4519,19 +4523,19 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J10" s="6">
         <v>0</v>
@@ -30018,64 +30022,64 @@
   <sheetData>
     <row r="1" spans="1:43" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="U1" s="12" t="s">
         <v>12</v>
@@ -30109,70 +30113,70 @@
     </row>
     <row r="2" spans="1:43" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="U2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W2" s="12" t="s">
         <v>16</v>
@@ -30266,7 +30270,7 @@
         <v>0</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30337,7 +30341,7 @@
         <v>0</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30408,7 +30412,7 @@
         <v>0</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30479,7 +30483,7 @@
         <v>0</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30550,7 +30554,7 @@
         <v>1</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30621,7 +30625,7 @@
         <v>1</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30692,7 +30696,7 @@
         <v>1</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30763,7 +30767,7 @@
         <v>1</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30834,7 +30838,7 @@
         <v>2</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30905,7 +30909,7 @@
         <v>2</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -30973,7 +30977,7 @@
         <v>2</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -31041,7 +31045,7 @@
         <v>2</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -31112,7 +31116,7 @@
         <v>3</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -31183,7 +31187,7 @@
         <v>3</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31254,7 +31258,7 @@
         <v>3</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31325,7 +31329,7 @@
         <v>3</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31396,7 +31400,7 @@
         <v>4</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31467,7 +31471,7 @@
         <v>4</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31538,7 +31542,7 @@
         <v>4</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31609,7 +31613,7 @@
         <v>4</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31680,7 +31684,7 @@
         <v>5</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31751,7 +31755,7 @@
         <v>5</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31822,7 +31826,7 @@
         <v>5</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31893,7 +31897,7 @@
         <v>5</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -31964,7 +31968,7 @@
         <v>6</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32032,7 +32036,7 @@
         <v>6</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32103,7 +32107,7 @@
         <v>6</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32174,7 +32178,7 @@
         <v>6</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32245,7 +32249,7 @@
         <v>7</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32316,7 +32320,7 @@
         <v>7</v>
       </c>
       <c r="W32" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32387,7 +32391,7 @@
         <v>7</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32455,7 +32459,7 @@
         <v>7</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32508,7 +32512,7 @@
         <v>8</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32579,7 +32583,7 @@
         <v>8</v>
       </c>
       <c r="W36" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32650,7 +32654,7 @@
         <v>8</v>
       </c>
       <c r="W37" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32721,7 +32725,7 @@
         <v>8</v>
       </c>
       <c r="W38" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32792,7 +32796,7 @@
         <v>9</v>
       </c>
       <c r="W39" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32863,7 +32867,7 @@
         <v>9</v>
       </c>
       <c r="W40" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -32934,7 +32938,7 @@
         <v>9</v>
       </c>
       <c r="W41" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -33005,7 +33009,7 @@
         <v>9</v>
       </c>
       <c r="W42" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -33531,7 +33535,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -33539,10 +33543,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved remaining bugs based on latest update"
</commit_message>
<xml_diff>
--- a/demos/public_good_experiment_prompt_template.xlsx
+++ b/demos/public_good_experiment_prompt_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raymondlow/Documents/talking-to-machines/talking-to-machines/demos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E6046A-CC52-C540-9C9E-79005B9469C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B646010-F450-CB43-994A-3D4CAFBF0CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1580" yWindow="-22560" windowWidth="36220" windowHeight="21460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experimental_setting" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="123">
   <si>
     <t>experimental_setting</t>
   </si>
@@ -111,16 +111,6 @@
   </si>
   <si>
     <t>Assume the role of a facilitator in a public good experiment.</t>
-  </si>
-  <si>
-    <t>Assume the role of a summariser in a public good experiment involving 4 participants. Each participant will start with an initial endowment of 10 tokens. During each round of the experiment, each participant is asked to decide how many tokens to contribute to a public account and how many to keep in their private account. The tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in the participants' private account will not be shared and remain private. 
-Example:
-A participant have 10 tokens. If that participant contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). The participant will keep the remaining 6 tokens in their private account. Contributions to the public account benefit everyone, including the participant. What they keep in their private account benefits only themselves. The total earnings for each round equal to private tokens kept + public tokens earned.
-At the end of each round, you are responsible for calculating the following information for each participant:
-- The total tokens contributed to the public account by all participants.
-- The participant's earnings from the public account.
-- The participant's private tokens kept from the round.
-- The participant's total earnings so far.</t>
   </si>
   <si>
     <t>Participant 1</t>
@@ -207,9 +197,6 @@
     <t>Please answer the following questions to ensure you understand the rules. If you contribute 5 tokens to the public account, how many total tokens will be in the public account before it is shared?</t>
   </si>
   <si>
-    <t>Please answer the following questions to ensure you understand the rules. If you contribute 5 tokens to the public account, how many total tokens will be in the public account before it is shared? {{response_options}}</t>
-  </si>
-  <si>
     <t>comprehension_qn_1</t>
   </si>
   <si>
@@ -222,9 +209,6 @@
     <t>Please answer the following questions to ensure you understand the rules. How are tokens from the public account distributed to group members?</t>
   </si>
   <si>
-    <t>Please answer the following questions to ensure you understand the rules. How are tokens from the public account distributed to group members? {{response_options}}</t>
-  </si>
-  <si>
     <t>comprehension_qn_2</t>
   </si>
   <si>
@@ -234,9 +218,6 @@
     <t>Please answer the following questions to ensure you understand the rules. If you keep all your tokens in your private account, what happens to the tokens in the public account?</t>
   </si>
   <si>
-    <t>Please answer the following questions to ensure you understand the rules. If you keep all your tokens in your private account, what happens to the tokens in the public account? {{response_options}}</t>
-  </si>
-  <si>
     <t>comprehension_qn_3</t>
   </si>
   <si>
@@ -246,29 +227,16 @@
     <t>How many tokens do you want to contribute to the public account? (Enter a number between 0 and 10)</t>
   </si>
   <si>
-    <t>{"Participant 1": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 2": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 3": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 4": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Summariser": "Calculate the following information for each participant in the following format:
-- The total tokens contributed to the public account by all participants:
-- The participant's earnings from the public account:
-- The participant's private tokens kept from the round:
-- The participant's total earnings so far:"}</t>
-  </si>
-  <si>
     <t>round_decision_1</t>
   </si>
   <si>
     <t>integer</t>
   </si>
   <si>
-    <t>range(11)</t>
-  </si>
-  <si>
     <t>round_decision_2</t>
   </si>
   <si>
     <t>round_decision_3</t>
-  </si>
-  <si>
-    <t>{"Participant 1": range(11), "Participant 2": range(11), "Participant 3": range(11), "Participant 4": range(11)}</t>
   </si>
   <si>
     <t>round_decision_4</t>
@@ -442,51 +410,76 @@
 </t>
   </si>
   <si>
-    <t>session assignment</t>
-  </si>
-  <si>
-    <t>Assume the role of a participant (Participant 1) in a public good experiment involving 3 other participants. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+    <t>(0,10)</t>
+  </si>
+  <si>
+    <t>{"Participant 1": (0,10), "Participant 2": (0,10), "Participant 3": (0,10), "Participant 4": (0,10)}</t>
+  </si>
+  <si>
+    <t>Assume the role of a summariser in a public good experiment involving 4 {{participant_label}}. Each {{participant_label}} will start with an initial endowment of 10 tokens. During each round of the experiment, each {{participant_label}} is asked to decide how many tokens to contribute to a public account and how many to keep in their private account. The tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in the {{participant_label}}s' private account will not be shared and remain private. 
+Example:
+A {{participant_label}} have 10 tokens. If that {{participant_label}} contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). The {{participant_label}} will keep the remaining 6 tokens in their private account. Contributions to the public account benefit everyone, including the {{participant_label}}. What they keep in their private account benefits only themselves. The total earnings for each round equal to private tokens kept + public tokens earned.
+At the end of each round, you are responsible for calculating the following information for each {{participant_label}}:
+- The total tokens contributed to the public account by all {{participant_label}}s.
+- The {{participant_label}}'s earnings from the public account.
+- The {{participant_label}}'s private tokens kept from the round.
+- The {{participant_label}}'s total earnings so far.</t>
+  </si>
+  <si>
+    <t>Assume the role of a {{participant_label}} (Participant 1) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
 Example: 
 You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
 At the end of each round, you will see:
-- The total tokens contributed to the public account by all participants.
+- The total tokens contributed to the public account by all {{participant_label}}s.
 - Your earnings from the public account.
 - Your private tokens kept from the round.
 - Your total earnings so far.
 Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
   </si>
   <si>
-    <t>Assume the role of a participant (Participant 2) in a public good experiment involving 3 other participants. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+    <t>Assume the role of a {{participant_label}} (Participant 2) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
 Example: 
 You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
 At the end of each round, you will see:
-- The total tokens contributed to the public account by all participants.
+- The total tokens contributed to the public account by all {{participant_label}}s.
 - Your earnings from the public account.
 - Your private tokens kept from the round.
 - Your total earnings so far.
 Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
   </si>
   <si>
-    <t>Assume the role of a participant (Participant 3) in a public good experiment involving 3 other participants. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+    <t>Assume the role of a {{participant_label}} (Participant 3) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
 Example: 
 You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
 At the end of each round, you will see:
-- The total tokens contributed to the public account by all participants.
+- The total tokens contributed to the public account by all {{participant_label}}s.
 - Your earnings from the public account.
 - Your private tokens kept from the round.
 - Your total earnings so far.
 Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
   </si>
   <si>
-    <t>Assume the role of a participant (Participant 4) in a public good experiment involving 3 other participants. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
+    <t>Assume the role of a {{participant_label}} (Participant 4) in a public good experiment involving 3 other {{participant_label}}s. You will start with an initial endowment of 10 tokens. During each round of the experiment, you must decide how many tokens to contribute to a public account and how many to keep in your private account. Tokens contributed to the public account will be multipled by a factor of 2 and distributed equally among all group members after each round. Tokens kept in your private account will not be shared and remain yours. 
 Example: 
 You have 10 tokens. If you contribute 4 tokens to the public account: These 4 tokens are doubled to 8 and shared equally among the group. Each group member receives 2 tokens (8 ÷ 4). You will keep the remaining 6 tokens in your private account. Contributions to the public account benefit everyone, including you. What you keep in your private account benefits only you. Your total earnings for each round equal to private tokens kept + public tokens earned.
 At the end of each round, you will see:
-- The total tokens contributed to the public account by all participants.
+- The total tokens contributed to the public account by all {{participant_label}}s.
 - Your earnings from the public account.
 - Your private tokens kept from the round.
 - Your total earnings so far.
 Answer any question that is posed to you in as much detail as possible and in the format required. Please provide a consistent and coherent response using all the demographic information provided about you. It is crucial for you to accurately replicate the response of a human subject that has the demographic profile you are provided. The human subject response will vary depending on their demographic profile. If you are unsure of an answer, provide a plausible response that is based on all of the information available to you. Do not include your name in your response.</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. If you contribute 5 tokens to the public account, how many total tokens will be in the public account before it is shared? {response_options}</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. How are tokens from the public account distributed to group members? {response_options}</t>
+  </si>
+  <si>
+    <t>Please answer the following questions to ensure you understand the rules. If you keep all your tokens in your private account, what happens to the tokens in the public account? {response_options}</t>
+  </si>
+  <si>
+    <t>{"Participant 1": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 2": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 3": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Participant 4": "How many tokens do you want to contribute to the public account? Enter a number between 0 and 10", "Summarizer": "Calculate the following information for each participant in the following format:\n- The total tokens contributed to the public account by all participants:\n- The participant's earnings from the public account:\n- The participant's private tokens kept from the round:\n- The participant's total earnings so far:"}</t>
   </si>
 </sst>
 </file>
@@ -773,7 +766,7 @@
   <dimension ref="A1:B1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -847,7 +840,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -863,7 +856,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -879,7 +872,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
@@ -887,7 +880,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B14" s="3">
         <v>42</v>
@@ -1891,9 +1884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2936,13 +2927,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="3" customWidth="1"/>
     <col min="2" max="4" width="10.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="3" customWidth="1"/>
     <col min="6" max="26" width="10.6640625" style="3" customWidth="1"/>
@@ -2967,42 +2956,42 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>110</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4008,8 +3997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L858"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4031,40 +4020,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4072,22 +4061,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4106,28 +4095,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
@@ -4144,7 +4133,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
@@ -4153,19 +4142,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
@@ -4182,7 +4171,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -4191,19 +4180,19 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
@@ -4220,7 +4209,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
@@ -4229,19 +4218,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
@@ -4258,7 +4247,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -4267,19 +4256,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="J7" s="3">
         <v>0</v>
@@ -4296,7 +4285,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
@@ -4305,19 +4294,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
@@ -4334,7 +4323,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>
@@ -4343,19 +4332,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="J9" s="3">
         <v>0</v>
@@ -4372,7 +4361,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2">
         <v>4</v>
@@ -4381,19 +4370,19 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
@@ -5264,7 +5253,7 @@
   <dimension ref="A1:AQ547"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5274,64 +5263,64 @@
   <sheetData>
     <row r="1" spans="1:43" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>12</v>
@@ -5365,70 +5354,70 @@
     </row>
     <row r="2" spans="1:43" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>16</v>
@@ -5522,7 +5511,7 @@
         <v>0</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -5593,7 +5582,7 @@
         <v>0</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -5664,7 +5653,7 @@
         <v>0</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -5735,7 +5724,7 @@
         <v>0</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -5806,7 +5795,7 @@
         <v>1</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -5877,7 +5866,7 @@
         <v>1</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -5948,7 +5937,7 @@
         <v>1</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -6019,7 +6008,7 @@
         <v>1</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -6090,7 +6079,7 @@
         <v>2</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -6161,7 +6150,7 @@
         <v>2</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -6230,7 +6219,7 @@
         <v>2</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -6299,7 +6288,7 @@
         <v>2</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -6370,7 +6359,7 @@
         <v>3</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:43" ht="16" x14ac:dyDescent="0.2">
@@ -6441,7 +6430,7 @@
         <v>3</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6512,7 +6501,7 @@
         <v>3</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6583,7 +6572,7 @@
         <v>3</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6654,7 +6643,7 @@
         <v>4</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6725,7 +6714,7 @@
         <v>4</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6796,7 +6785,7 @@
         <v>4</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6867,7 +6856,7 @@
         <v>4</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6938,7 +6927,7 @@
         <v>5</v>
       </c>
       <c r="W23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7009,7 +6998,7 @@
         <v>5</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7080,7 +7069,7 @@
         <v>5</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7151,7 +7140,7 @@
         <v>5</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7222,7 +7211,7 @@
         <v>6</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7291,7 +7280,7 @@
         <v>6</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7362,7 +7351,7 @@
         <v>6</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7433,7 +7422,7 @@
         <v>6</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7504,7 +7493,7 @@
         <v>7</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7575,7 +7564,7 @@
         <v>7</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7646,7 +7635,7 @@
         <v>7</v>
       </c>
       <c r="W33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7715,7 +7704,7 @@
         <v>7</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7774,7 +7763,7 @@
         <v>8</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7845,7 +7834,7 @@
         <v>8</v>
       </c>
       <c r="W36" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7916,7 +7905,7 @@
         <v>8</v>
       </c>
       <c r="W37" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -7987,7 +7976,7 @@
         <v>8</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -8058,7 +8047,7 @@
         <v>9</v>
       </c>
       <c r="W39" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -8129,7 +8118,7 @@
         <v>9</v>
       </c>
       <c r="W40" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -8200,7 +8189,7 @@
         <v>9</v>
       </c>
       <c r="W41" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -8271,7 +8260,7 @@
         <v>9</v>
       </c>
       <c r="W42" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8786,8 +8775,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8800,7 +8789,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -8808,10 +8797,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>